<commit_message>
fix: error and run Ragar
</commit_message>
<xml_diff>
--- a/testing/politifact_datasets/cleaned_statements.xlsx
+++ b/testing/politifact_datasets/cleaned_statements.xlsx
@@ -770,7 +770,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -2327,7 +2327,7 @@
         <v>110</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="19.5">
       <c r="A85" s="3">
         <v>10662</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>106</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="19.5">
       <c r="A86" s="3">
         <v>13762</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>156</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="19.5">
       <c r="A87" s="3">
         <v>22506</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>110</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="19.5">
       <c r="A88" s="3">
         <v>17491</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>124</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="19.5">
       <c r="A89" s="3">
         <v>16726</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>110</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="19.5">
       <c r="A90" s="3">
         <v>10702</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>161</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="19.5">
       <c r="A91" s="3">
         <v>846</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>163</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="19.5">
       <c r="A92" s="3">
         <v>12685</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>165</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="19.5">
       <c r="A93" s="3">
         <v>13443</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>167</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="19.5">
       <c r="A94" s="3">
         <v>23684</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>169</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="19.5">
       <c r="A95" s="3">
         <v>23326</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>115</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="19.5">
       <c r="A96" s="3">
         <v>10892</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="19.5">
       <c r="A97" s="3">
         <v>22294</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>106</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="19.5">
       <c r="A98" s="3">
         <v>15284</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>174</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="19.5">
       <c r="A99" s="3">
         <v>18107</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>110</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="19.5">
       <c r="A100" s="3">
         <v>13869</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>177</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="19.5">
       <c r="A101" s="3">
         <v>5088</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>179</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="19.5">
       <c r="A102" s="3">
         <v>329</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="19.5">
       <c r="A103" s="3">
         <v>13739</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>182</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="19.5">
       <c r="A104" s="3">
         <v>5225</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>184</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="19.5">
       <c r="A105" s="3">
         <v>13921</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>186</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="19.5">
       <c r="A106" s="3">
         <v>12067</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>188</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="19.5">
       <c r="A107" s="3">
         <v>9858</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>190</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="19.5">
       <c r="A108" s="3">
         <v>6285</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>69</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="19.5">
       <c r="A109" s="3">
         <v>2293</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="19.5">
       <c r="A110" s="3">
         <v>4716</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>117</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="19.5">
       <c r="A111" s="3">
         <v>1609</v>
       </c>

</xml_diff>